<commit_message>
updated the example files to latest figure6 and OBCS release version
</commit_message>
<xml_diff>
--- a/docs/user/example/Figure3 term list.xlsx
+++ b/docs/user/example/Figure3 term list.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="165" windowWidth="22995" windowHeight="9915"/>
+    <workbookView xWindow="480" yWindow="160" windowWidth="23000" windowHeight="13820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,9 +30,6 @@
     <t>data collection from experiment</t>
   </si>
   <si>
-    <t>set of data set</t>
-  </si>
-  <si>
     <t>background correction data transformation</t>
   </si>
   <si>
@@ -140,6 +142,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0000295</t>
+  </si>
+  <si>
+    <t>data matrix</t>
   </si>
 </sst>
 </file>
@@ -505,26 +510,26 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47.5" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -532,162 +537,167 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>